<commit_message>
Feat: developed send mail function
</commit_message>
<xml_diff>
--- a/KDT_HWrepo_Week3/email_list.xlsx
+++ b/KDT_HWrepo_Week3/email_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeong-isu/PycharmProjects/23th-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeong-isu/dev/KDT_HWrepo/KDT_HWrepo_Week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B269B1-3438-5F45-9B76-83A1F4273BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB8FB86-579D-4E4B-B865-436F0EB6F200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11840" yWindow="5900" windowWidth="21760" windowHeight="15100" xr2:uid="{7BB770C9-AE3B-2948-BBB2-9397C3D131F6}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>email_list</t>
   </si>
@@ -58,13 +49,30 @@
   </si>
   <si>
     <t>masterofflash@nate.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정이수</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>mustdoit2020@gmail.com</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +102,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -117,12 +141,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -135,9 +162,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E60F9E9-A98D-0845-BC13-4C9965187C6D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -497,8 +528,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{EC5A3BFF-657F-6245-ADBA-E0A2FABF00EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>